<commit_message>
Added info to 0x1DC and 0x55B
Added the latest findings in EV-CAN reverse engineering. Updated info on frame 0x55B for what the SOC actually affects, and most importantly, added information about pairing in a new battery in frame 0x1DC (24/30/40kWh upgrades!)
</commit_message>
<xml_diff>
--- a/canmsgs.xlsx
+++ b/canmsgs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dos001\Documents\Leaf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37AEBE6-4036-41CE-B3D7-3B09B7717C4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16062B30-73B0-4BF8-8418-7FD584D4AA37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="14025" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,14 @@
   <definedNames>
     <definedName name="NamedRange1">'370Z from brad370'!$A$1:$T$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -82,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3703" uniqueCount="1223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3705" uniqueCount="1224">
   <si>
     <t>Signal name</t>
   </si>
@@ -3815,9 +3822,6 @@
     <t>Lithium Battery Controler aka "BMS/LBC"</t>
   </si>
   <si>
-    <t>Probably Lithium Battery Controller "LBC/BMS"</t>
-  </si>
-  <si>
     <t>Lithium Battery Controller "LBC/BMS"</t>
   </si>
   <si>
@@ -3830,10 +3834,16 @@
     <t>The indicated temperature on the instrument cluster is controlled by another muxed field, when 0x5C0 is 0x40, the indicated temperature is controlled by the 3rd byte of 0x5C0. This mux has 3 values, on this car all 3 are similar in the 3rd byte, but only the when the mux is 0x40 does the 3rd byte control the temperature in the instrument cluster.</t>
   </si>
   <si>
-    <t>59..8c ---SOC is stored in first 10bits of 55b, does not affect charge bars</t>
-  </si>
-  <si>
     <t>SOC (State of charge)</t>
+  </si>
+  <si>
+    <t>59..8c ---SOC is stored in first 10bits of 55b, does not affect charge bars. The VCM actually has an internal SOC% which it ONLY updates upwards at end of charge.</t>
+  </si>
+  <si>
+    <t>BATTERY PAIRING DATA</t>
+  </si>
+  <si>
+    <t>Just a hint on those pursuing 40/30/24kWh translations: We are suspecting the 'pairing' tool just changes 0x1DC bytes 5 and 6 (as in: third and second to last bytes). Beyond that, there are some very minor differences between the LBCs, but the most important bits are in the same place and work the same way. You get a P3183 DTC when swapping batteries.</t>
   </si>
 </sst>
 </file>
@@ -22953,8 +22963,8 @@
   <dimension ref="A1:K209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A149" sqref="A149:A158"/>
+      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24026,6 +24036,9 @@
       <c r="F49" s="25">
         <v>0</v>
       </c>
+      <c r="H49" s="264" t="s">
+        <v>1222</v>
+      </c>
       <c r="J49" s="26" t="s">
         <v>245</v>
       </c>
@@ -24045,6 +24058,9 @@
       </c>
       <c r="F50" s="25">
         <v>0</v>
+      </c>
+      <c r="H50" s="264" t="s">
+        <v>1223</v>
       </c>
       <c r="J50" s="26" t="s">
         <v>246</v>
@@ -26179,7 +26195,7 @@
       </c>
       <c r="G149" s="33"/>
       <c r="H149" s="299" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="I149" s="33"/>
       <c r="J149" s="86" t="s">
@@ -26774,7 +26790,7 @@
         <v>1213</v>
       </c>
       <c r="K177" s="284" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="178" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -26893,10 +26909,10 @@
         <v>0</v>
       </c>
       <c r="H183" s="27" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="J183" s="26" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="K183" s="285"/>
     </row>
@@ -27172,7 +27188,7 @@
         <v>633</v>
       </c>
       <c r="K196" s="284" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="197" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -27227,7 +27243,7 @@
         <v>0</v>
       </c>
       <c r="H199" s="264" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="J199" s="26" t="s">
         <v>635</v>
@@ -27562,8 +27578,8 @@
   <dimension ref="A1:K477"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B465" sqref="B465:B473"/>
+      <pane ySplit="2" topLeftCell="A438" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>